<commit_message>
Update task list to reflect different tactic for templates
</commit_message>
<xml_diff>
--- a/docs/Task List.xlsx
+++ b/docs/Task List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahardy/omscs/ahardy30-proposal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahardy/Desktop/storypixies/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303AE2FD-E05F-CF4B-A199-186FBAF5253A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AC4715-71F3-914B-BBC3-CD89C13A453D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="460" windowWidth="24880" windowHeight="16600" xr2:uid="{950462DB-7968-1E4A-B5F0-08A117BB4217}"/>
+    <workbookView xWindow="3020" yWindow="460" windowWidth="24880" windowHeight="16580" xr2:uid="{950462DB-7968-1E4A-B5F0-08A117BB4217}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="92">
   <si>
     <t>Week</t>
   </si>
@@ -286,6 +286,21 @@
   </si>
   <si>
     <t>Total Hours</t>
+  </si>
+  <si>
+    <t>Template Editor</t>
+  </si>
+  <si>
+    <t>New Templates can be created</t>
+  </si>
+  <si>
+    <t>Stories from Template</t>
+  </si>
+  <si>
+    <t>New Stories can be created from a template or another story</t>
+  </si>
+  <si>
+    <t>Templates and New Stories</t>
   </si>
 </sst>
 </file>
@@ -329,7 +344,7 @@
       <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,6 +384,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -467,24 +494,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -504,6 +513,39 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -819,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B600A05F-AF66-904D-8694-75C07305FC59}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -831,6 +873,8 @@
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickBot="1">
@@ -851,13 +895,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="35" customHeight="1" thickBot="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:5" ht="52" thickBot="1">
       <c r="A3" s="1" t="s">
@@ -935,23 +979,23 @@
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="17" thickBot="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10">
         <f>SUM(D3:D7)</f>
         <v>10.25</v>
       </c>
-      <c r="E8" s="15"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="31" customHeight="1" thickBot="1">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:5" ht="35" thickBot="1">
       <c r="A10" s="3" t="s">
@@ -1014,23 +1058,23 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="17" thickBot="1">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10">
         <f>SUM(D10:D13)</f>
         <v>13.25</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" ht="37" customHeight="1" thickBot="1">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" ht="35" thickBot="1">
       <c r="A16" s="1" t="s">
@@ -1093,23 +1137,23 @@
       <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" ht="17" thickBot="1">
-      <c r="A20" s="17"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16">
+      <c r="A20" s="11"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10">
         <f>SUM(D16:D19)</f>
         <v>10.25</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" ht="17" thickBot="1">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:5" ht="35" thickBot="1">
       <c r="A22" s="1" t="s">
@@ -1172,23 +1216,23 @@
       <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" ht="17" thickBot="1">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="16">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10">
         <f>SUM(D22:D25)</f>
         <v>11.25</v>
       </c>
-      <c r="E26" s="15"/>
+      <c r="E26" s="9"/>
     </row>
     <row r="27" spans="1:5" ht="17" thickBot="1">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="18"/>
     </row>
     <row r="28" spans="1:5" ht="69" thickBot="1">
       <c r="A28" s="1" t="s">
@@ -1220,18 +1264,18 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="35" thickBot="1">
+    <row r="30" spans="1:5" ht="18" thickBot="1">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D30" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E30" s="7"/>
     </row>
@@ -1251,104 +1295,171 @@
       <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" ht="17" thickBot="1">
-      <c r="A32" s="14"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="10">
         <f>SUM(D28:D31)</f>
-        <v>12.25</v>
-      </c>
-      <c r="E32" s="15"/>
-    </row>
-    <row r="33" spans="1:5" ht="17" thickBot="1">
-      <c r="A33" s="8" t="s">
+        <v>13.25</v>
+      </c>
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:10" ht="17" customHeight="1" thickBot="1">
+      <c r="A33" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" spans="1:5" ht="69" thickBot="1">
-      <c r="A34" s="1" t="s">
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="18"/>
+    </row>
+    <row r="34" spans="1:10" ht="69" thickBot="1">
+      <c r="A34" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="26">
         <v>4</v>
       </c>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" ht="35" thickBot="1">
-      <c r="A35" s="1" t="s">
+      <c r="E34" s="26"/>
+      <c r="F34" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="G34" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I34" s="7">
+        <v>4</v>
+      </c>
+      <c r="J34" s="7"/>
+    </row>
+    <row r="35" spans="1:10" ht="35" thickBot="1">
+      <c r="A35" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="26">
         <v>4</v>
       </c>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="1:5" ht="18" thickBot="1">
-      <c r="A36" s="1" t="s">
+      <c r="E35" s="26"/>
+      <c r="F35" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="7">
-        <v>3</v>
-      </c>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="1:5" ht="35" thickBot="1">
-      <c r="A37" s="1" t="s">
+      <c r="G35" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I35" s="7">
+        <v>4</v>
+      </c>
+      <c r="J35" s="7"/>
+    </row>
+    <row r="36" spans="1:10" ht="35" thickBot="1">
+      <c r="A36" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B36" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="26">
+        <v>2</v>
+      </c>
+      <c r="E36" s="26"/>
+      <c r="F36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I36" s="7">
+        <v>2</v>
+      </c>
+      <c r="J36" s="7"/>
+    </row>
+    <row r="37" spans="1:10" ht="35" thickBot="1">
+      <c r="A37" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="26">
         <v>0.25</v>
       </c>
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="1:5" ht="17" thickBot="1">
-      <c r="A38" s="14"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="16">
+      <c r="E37" s="26"/>
+      <c r="F37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I37" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="J37" s="7"/>
+    </row>
+    <row r="38" spans="1:10" ht="17" thickBot="1">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="10">
         <f>SUM(D34:D37)</f>
-        <v>11.25</v>
-      </c>
-      <c r="E38" s="15"/>
-    </row>
-    <row r="39" spans="1:5" ht="17" thickBot="1">
-      <c r="A39" s="8" t="s">
+        <v>10.25</v>
+      </c>
+      <c r="E38" s="9"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="10">
+        <f>SUM(I34:I37)</f>
+        <v>10.25</v>
+      </c>
+      <c r="J38" s="9"/>
+    </row>
+    <row r="39" spans="1:10" ht="17" thickBot="1">
+      <c r="A39" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" spans="1:5" ht="52" thickBot="1">
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" spans="1:10" ht="52" thickBot="1">
       <c r="A40" s="1" t="s">
         <v>65</v>
       </c>
@@ -1363,7 +1474,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="35" thickBot="1">
+    <row r="41" spans="1:10" ht="35" thickBot="1">
       <c r="A41" s="1" t="s">
         <v>65</v>
       </c>
@@ -1378,7 +1489,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" ht="35" thickBot="1">
+    <row r="42" spans="1:10" ht="35" thickBot="1">
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
@@ -1393,7 +1504,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" ht="35" thickBot="1">
+    <row r="43" spans="1:10" ht="35" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>65</v>
       </c>
@@ -1408,26 +1519,26 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" ht="17" thickBot="1">
-      <c r="A44" s="17"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16">
+    <row r="44" spans="1:10" ht="17" thickBot="1">
+      <c r="A44" s="11"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10">
         <f>SUM(D40:D43)</f>
         <v>11.25</v>
       </c>
-      <c r="E44" s="16"/>
-    </row>
-    <row r="45" spans="1:5" ht="17" thickBot="1">
-      <c r="A45" s="8" t="s">
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45" spans="1:10" ht="17" thickBot="1">
+      <c r="A45" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" spans="1:5" ht="52" thickBot="1">
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="18"/>
+    </row>
+    <row r="46" spans="1:10" ht="52" thickBot="1">
       <c r="A46" s="1" t="s">
         <v>66</v>
       </c>
@@ -1442,7 +1553,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" ht="52" thickBot="1">
+    <row r="47" spans="1:10" ht="52" thickBot="1">
       <c r="A47" s="1" t="s">
         <v>66</v>
       </c>
@@ -1457,7 +1568,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="35" thickBot="1">
+    <row r="48" spans="1:10" ht="35" thickBot="1">
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
@@ -1488,23 +1599,23 @@
       <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5" ht="17" thickBot="1">
-      <c r="A50" s="17"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16">
+      <c r="A50" s="11"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10">
         <f>SUM(D46:D49)</f>
         <v>11.25</v>
       </c>
-      <c r="E50" s="16"/>
+      <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5" ht="17" thickBot="1">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="10"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="18"/>
     </row>
     <row r="52" spans="1:5" ht="52" thickBot="1">
       <c r="A52" s="1" t="s">
@@ -1552,32 +1663,33 @@
       <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5" ht="18" thickBot="1">
-      <c r="A55" s="17"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16" t="s">
+      <c r="A55" s="11"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D55" s="16">
+      <c r="D55" s="10">
         <f>SUM(D52:D54)</f>
         <v>9.5</v>
       </c>
-      <c r="E55" s="16"/>
+      <c r="E55" s="10"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="20"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="21" t="s">
+      <c r="A56" s="14"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D56" s="18">
+      <c r="D56" s="12">
         <f>SUM(D8,D14,D20,D26,D32,D38,D44,D50,D55)</f>
         <v>100.5</v>
       </c>
-      <c r="E56" s="19"/>
+      <c r="E56" s="13"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="F33:J33"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A39:E39"/>
     <mergeCell ref="A45:E45"/>

</xml_diff>

<commit_message>
Updating task list to reflect changed priorities
</commit_message>
<xml_diff>
--- a/docs/Task List.xlsx
+++ b/docs/Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahardy/Desktop/storypixies/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AC4715-71F3-914B-BBC3-CD89C13A453D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF431D3C-B596-5947-AEF7-D65B416263D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="460" windowWidth="24880" windowHeight="16580" xr2:uid="{950462DB-7968-1E4A-B5F0-08A117BB4217}"/>
+    <workbookView xWindow="100" yWindow="2980" windowWidth="24880" windowHeight="13620" xr2:uid="{950462DB-7968-1E4A-B5F0-08A117BB4217}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t>Creator Dive</t>
   </si>
   <si>
-    <t xml:space="preserve">Creator Part II </t>
-  </si>
-  <si>
     <t>Functionaity title page editor</t>
   </si>
   <si>
@@ -301,6 +298,9 @@
   </si>
   <si>
     <t>Templates and New Stories</t>
+  </si>
+  <si>
+    <t>Creator part II</t>
   </si>
 </sst>
 </file>
@@ -514,6 +514,12 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -523,6 +529,15 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -530,21 +545,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B600A05F-AF66-904D-8694-75C07305FC59}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -895,13 +895,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="35" customHeight="1" thickBot="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
     </row>
     <row r="3" spans="1:5" ht="52" thickBot="1">
       <c r="A3" s="1" t="s">
@@ -989,13 +989,13 @@
       <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="31" customHeight="1" thickBot="1">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
     </row>
     <row r="10" spans="1:5" ht="35" thickBot="1">
       <c r="A10" s="3" t="s">
@@ -1068,13 +1068,13 @@
       <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" ht="37" customHeight="1" thickBot="1">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
     </row>
     <row r="16" spans="1:5" ht="35" thickBot="1">
       <c r="A16" s="1" t="s">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="103" thickBot="1">
+    <row r="17" spans="1:10" ht="103" thickBot="1">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1099,14 +1099,14 @@
         <v>10</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" s="7">
         <v>5</v>
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" ht="35" thickBot="1">
+    <row r="18" spans="1:10" ht="35" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" ht="35" thickBot="1">
+    <row r="19" spans="1:10" ht="35" thickBot="1">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" ht="17" thickBot="1">
+    <row r="20" spans="1:10" ht="17" thickBot="1">
       <c r="A20" s="11"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -1146,16 +1146,16 @@
       </c>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="1:5" ht="17" thickBot="1">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:10" ht="17" thickBot="1">
+      <c r="A21" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="18"/>
-    </row>
-    <row r="22" spans="1:5" ht="35" thickBot="1">
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="1:10" ht="35" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" ht="69" thickBot="1">
+    <row r="23" spans="1:10" ht="69" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="18" thickBot="1">
+    <row r="24" spans="1:10" ht="18" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" ht="35" thickBot="1">
+    <row r="25" spans="1:10" ht="35" thickBot="1">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" ht="17" thickBot="1">
+    <row r="26" spans="1:10" ht="17" thickBot="1">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -1225,61 +1225,74 @@
       </c>
       <c r="E26" s="9"/>
     </row>
-    <row r="27" spans="1:5" ht="17" thickBot="1">
-      <c r="A27" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="18"/>
-    </row>
-    <row r="28" spans="1:5" ht="69" thickBot="1">
+    <row r="27" spans="1:10" ht="17" customHeight="1" thickBot="1">
+      <c r="A27" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:10" ht="69" thickBot="1">
       <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="D28" s="7">
         <v>4</v>
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="52" thickBot="1">
+    <row r="29" spans="1:10" ht="52" thickBot="1">
       <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="D29" s="7">
         <v>6</v>
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="18" thickBot="1">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:10" ht="35" thickBot="1">
+      <c r="A30" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="17">
+        <v>2</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="H30" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="7">
+      <c r="I30" s="7">
         <v>3</v>
       </c>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="1:5" ht="35" thickBot="1">
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:10" ht="35" thickBot="1">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
@@ -1294,54 +1307,54 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" ht="17" thickBot="1">
+    <row r="32" spans="1:10" ht="17" thickBot="1">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="10">
-        <f>SUM(D28:D31)</f>
+        <f>SUM(D28,D29,I30,D31)</f>
         <v>13.25</v>
       </c>
       <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:10" ht="17" customHeight="1" thickBot="1">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="18"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="69" thickBot="1">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="C34" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" s="26">
+      <c r="D34" s="17">
         <v>4</v>
       </c>
-      <c r="E34" s="26"/>
+      <c r="E34" s="17"/>
       <c r="F34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G34" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H34" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="I34" s="7">
         <v>4</v>
@@ -1349,27 +1362,27 @@
       <c r="J34" s="7"/>
     </row>
     <row r="35" spans="1:10" ht="35" thickBot="1">
-      <c r="A35" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="26" t="s">
+      <c r="A35" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="26">
+      <c r="D35" s="17">
         <v>4</v>
       </c>
-      <c r="E35" s="26"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G35" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H35" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="I35" s="7">
         <v>4</v>
@@ -1377,27 +1390,27 @@
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:10" ht="35" thickBot="1">
-      <c r="A36" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36" s="26" t="s">
+      <c r="A36" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="17">
+        <v>3</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" s="26">
-        <v>2</v>
-      </c>
-      <c r="E36" s="26"/>
-      <c r="F36" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="I36" s="7">
         <v>2</v>
@@ -1405,69 +1418,48 @@
       <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:10" ht="35" thickBot="1">
-      <c r="A37" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="26" t="s">
+      <c r="A37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="26">
+      <c r="D37" s="7">
         <v>0.25</v>
       </c>
-      <c r="E37" s="26"/>
-      <c r="F37" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I37" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="J37" s="7"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:10" ht="17" thickBot="1">
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
       <c r="D38" s="10">
-        <f>SUM(D34:D37)</f>
+        <f>SUM(I34,I35,I36,D37)</f>
         <v>10.25</v>
       </c>
       <c r="E38" s="9"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="10">
-        <f>SUM(I34:I37)</f>
-        <v>10.25</v>
-      </c>
-      <c r="J38" s="9"/>
     </row>
     <row r="39" spans="1:10" ht="17" thickBot="1">
-      <c r="A39" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="18"/>
+      <c r="A39" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="20"/>
     </row>
     <row r="40" spans="1:10" ht="52" thickBot="1">
       <c r="A40" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="D40" s="7">
         <v>8</v>
@@ -1476,13 +1468,13 @@
     </row>
     <row r="41" spans="1:10" ht="35" thickBot="1">
       <c r="A41" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="D41" s="7">
         <v>2</v>
@@ -1491,13 +1483,13 @@
     </row>
     <row r="42" spans="1:10" ht="35" thickBot="1">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>81</v>
       </c>
       <c r="D42" s="7">
         <v>1</v>
@@ -1506,10 +1498,10 @@
     </row>
     <row r="43" spans="1:10" ht="35" thickBot="1">
       <c r="A43" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>8</v>
@@ -1530,23 +1522,23 @@
       <c r="E44" s="10"/>
     </row>
     <row r="45" spans="1:10" ht="17" thickBot="1">
-      <c r="A45" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="18"/>
+      <c r="A45" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="20"/>
     </row>
     <row r="46" spans="1:10" ht="52" thickBot="1">
       <c r="A46" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="C46" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="D46" s="7">
         <v>6</v>
@@ -1555,13 +1547,13 @@
     </row>
     <row r="47" spans="1:10" ht="52" thickBot="1">
       <c r="A47" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="D47" s="7">
         <v>4</v>
@@ -1570,13 +1562,13 @@
     </row>
     <row r="48" spans="1:10" ht="35" thickBot="1">
       <c r="A48" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="D48" s="7">
         <v>1</v>
@@ -1585,10 +1577,10 @@
     </row>
     <row r="49" spans="1:5" ht="35" thickBot="1">
       <c r="A49" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>8</v>
@@ -1609,23 +1601,23 @@
       <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5" ht="17" thickBot="1">
-      <c r="A51" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="18"/>
+      <c r="A51" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="20"/>
     </row>
     <row r="52" spans="1:5" ht="52" thickBot="1">
       <c r="A52" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="C52" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="D52" s="7">
         <v>1.5</v>
@@ -1634,13 +1626,13 @@
     </row>
     <row r="53" spans="1:5" ht="18" thickBot="1">
       <c r="A53" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B53" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="D53" s="7">
         <v>5</v>
@@ -1649,13 +1641,13 @@
     </row>
     <row r="54" spans="1:5" ht="35" thickBot="1">
       <c r="A54" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="D54" s="2">
         <v>3</v>
@@ -1678,7 +1670,7 @@
       <c r="A56" s="14"/>
       <c r="B56" s="13"/>
       <c r="C56" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D56" s="12">
         <f>SUM(D8,D14,D20,D26,D32,D38,D44,D50,D55)</f>
@@ -1689,16 +1681,16 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="10">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A27:E27"/>
     <mergeCell ref="F33:J33"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A39:E39"/>
     <mergeCell ref="A45:E45"/>
     <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A27:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>